<commit_message>
Added test for generated json
</commit_message>
<xml_diff>
--- a/json_generator/test/test.xlsx
+++ b/json_generator/test/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/repos/robot_helpers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/repos/robot_helpers/json_generator/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E337DA1-A61F-ED40-879F-67BE3041C364}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55085C06-CA8B-0448-BBD6-60764680E041}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="1780" windowWidth="27640" windowHeight="16940" xr2:uid="{3C577023-E956-7546-9CF2-4BAFC427EDAE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Key - Do not translate!</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Unelma</t>
+  </si>
+  <si>
+    <t>Một chìa khóa khác</t>
   </si>
 </sst>
 </file>
@@ -809,10 +812,10 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1079,25 +1082,28 @@
       <c r="D16" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="F16" s="18" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:F1048576">
-    <cfRule type="containsBlanks" dxfId="0" priority="398">
+    <cfRule type="containsBlanks" dxfId="3" priority="398">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="containsBlanks" dxfId="3" priority="391">
+    <cfRule type="containsBlanks" dxfId="2" priority="391">
       <formula>LEN(TRIM(A8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="containsBlanks" dxfId="2" priority="110">
+    <cfRule type="containsBlanks" dxfId="1" priority="110">
       <formula>LEN(TRIM(F6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:D7">
-    <cfRule type="containsBlanks" dxfId="1" priority="71">
+    <cfRule type="containsBlanks" dxfId="0" priority="71">
       <formula>LEN(TRIM(C7))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>